<commit_message>
Curso de Javascript e Dataset Fut
</commit_message>
<xml_diff>
--- a/Excel/Controle-Mercado-inicial.xlsx
+++ b/Excel/Controle-Mercado-inicial.xlsx
@@ -276,7 +276,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Retângulo 1"/>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -335,24 +337,26 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Retângulo 2"/>
+        <xdr:cNvPr id="3" name="Retângulo 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3057525" y="590550"/>
+          <a:off x="3048000" y="590550"/>
           <a:ext cx="1771650" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -403,25 +407,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Retângulo 3"/>
+        <xdr:cNvPr id="4" name="Retângulo 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5495925" y="581025"/>
+          <a:off x="5419725" y="600075"/>
           <a:ext cx="1771650" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -472,25 +478,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Retângulo 4"/>
+        <xdr:cNvPr id="5" name="Retângulo 4">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7934325" y="571500"/>
+          <a:off x="7781925" y="590550"/>
           <a:ext cx="1771650" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -541,25 +549,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Retângulo 5"/>
+        <xdr:cNvPr id="6" name="Retângulo 5">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10372725" y="552450"/>
+          <a:off x="12411075" y="619125"/>
           <a:ext cx="1771650" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -610,25 +620,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Retângulo 6"/>
+        <xdr:cNvPr id="7" name="Retângulo 6">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12792075" y="561975"/>
+          <a:off x="10134600" y="600075"/>
           <a:ext cx="1771650" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -935,7 +947,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -960,9 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1203,9 +1213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1231,9 +1239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>